<commit_message>
Se corrigió dividir las constantes de algunos compuestos en dos archivos, así como sus archivos de verificaciones. Se eliminó el uso de eval en la función Escribir Excel. Se quitó código redundante en el programa principal y se añadieron medidores de velocidad.
</commit_message>
<xml_diff>
--- a/VerificacionCompuestos/PruebaSalida.xlsx
+++ b/VerificacionCompuestos/PruebaSalida.xlsx
@@ -8,19 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pamem\OneDrive - UNIVERSIDAD NACIONAL AUTÓNOMA DE MÉXICO\Programación\Matemáticas\Matlab\Proyecto Ana\VerificacionCompuestos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BADCB144-4A54-4B7F-B030-80060DBFF72B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{446EB641-2213-4A4F-9B78-0CA18705EB77}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16389" windowHeight="12163" firstSheet="3" activeTab="7" xr2:uid="{DFE9CF76-3B7E-424E-B8C9-935158DEB7B1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16389" windowHeight="12163" firstSheet="2" activeTab="6" xr2:uid="{52623749-0325-4C4F-96ED-C1BE82E86AD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Salida" sheetId="2" r:id="rId2"/>
+    <sheet name="DOLCALSIL" sheetId="2" r:id="rId2"/>
     <sheet name="ArcillaDOLSIL" sheetId="3" r:id="rId3"/>
-    <sheet name="DOLCALSIL" sheetId="4" r:id="rId4"/>
-    <sheet name="FI2CaCOCaCODOL" sheetId="5" r:id="rId5"/>
-    <sheet name="FI2DOLDOLCaCO" sheetId="6" r:id="rId6"/>
-    <sheet name="GYPANHDOL" sheetId="7" r:id="rId7"/>
-    <sheet name="SalSIL" sheetId="8" r:id="rId8"/>
+    <sheet name="FI2CaCOCaCODOL" sheetId="4" r:id="rId4"/>
+    <sheet name="FI2DOLDOLCaCO" sheetId="5" r:id="rId5"/>
+    <sheet name="GYPANHDOL" sheetId="6" r:id="rId6"/>
+    <sheet name="SalSIL" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -32,9 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
-    <t>GYPANDHOL</t>
+    <t>DOLCALSIL</t>
   </si>
   <si>
     <t>No.</t>
@@ -47,9 +46,6 @@
   </si>
   <si>
     <t>ArcillaDOLSIL</t>
-  </si>
-  <si>
-    <t>DOLCALSIL</t>
   </si>
   <si>
     <t>FI2CaCOCaCODOL</t>
@@ -412,7 +408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7402BAB-5CFE-42B8-B3DC-505130D99792}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6CE6A9-6459-424F-982D-642CA999D7F7}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -424,11 +420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDA9E72-46E5-4D23-A423-C99BC559664A}">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9271C35C-AE20-460F-B9B2-19472DF34D0C}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C16"/>
+      <selection sqref="A1:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -451,156 +447,277 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>0.47880839539607317</v>
+        <v>0.5535201807412834</v>
       </c>
       <c r="C3">
-        <v>0.78719634394041993</v>
+        <v>0.79824204677291311</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>227</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>0.5222508687366888</v>
+        <v>0.55514309663513361</v>
       </c>
       <c r="C4">
-        <v>0.77962392108508027</v>
+        <v>0.79375943000838234</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>267</v>
+        <v>39</v>
       </c>
       <c r="B5">
-        <v>0.50399322362052268</v>
+        <v>0.54480670997036007</v>
       </c>
       <c r="C5">
-        <v>0.71038661665053238</v>
+        <v>0.79284543103991922</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>278</v>
+        <v>40</v>
       </c>
       <c r="B6">
-        <v>0.51686067442697714</v>
+        <v>0.55123199999999994</v>
       </c>
       <c r="C6">
-        <v>0.76248049921996897</v>
+        <v>0.79430015999999992</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>279</v>
+        <v>49</v>
       </c>
       <c r="B7">
-        <v>0.51350378105869643</v>
+        <v>0.56088340628730604</v>
       </c>
       <c r="C7">
-        <v>0.76033969511463229</v>
+        <v>0.79514060220188354</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>280</v>
+        <v>50</v>
       </c>
       <c r="B8">
-        <v>0.51304767070451396</v>
+        <v>0.56504494976203068</v>
       </c>
       <c r="C8">
-        <v>0.75942867474236131</v>
+        <v>0.79988696456901109</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>281</v>
+        <v>51</v>
       </c>
       <c r="B9">
-        <v>0.51346118942464769</v>
+        <v>0.56937767533750416</v>
       </c>
       <c r="C9">
-        <v>0.75693266380301294</v>
+        <v>0.80036088244978598</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>282</v>
+        <v>52</v>
       </c>
       <c r="B10">
-        <v>0.5139410837677294</v>
+        <v>0.57145666710371057</v>
       </c>
       <c r="C10">
-        <v>0.75307128136743839</v>
+        <v>0.79708732135833227</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>283</v>
+        <v>78</v>
       </c>
       <c r="B11">
-        <v>0.51474335638878776</v>
+        <v>0.5711252653927813</v>
       </c>
       <c r="C11">
-        <v>0.74931258342434159</v>
+        <v>0.80882228050455851</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>341</v>
+        <v>113</v>
       </c>
       <c r="B12">
-        <v>0.51855864074348601</v>
+        <v>0.55115106052767715</v>
       </c>
       <c r="C12">
-        <v>0.76361024003649025</v>
+        <v>0.79123706673564398</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13">
-        <v>342</v>
+        <v>133</v>
       </c>
       <c r="B13">
-        <v>0.51224593209841784</v>
+        <v>0.56151945645460155</v>
       </c>
       <c r="C13">
-        <v>0.74628568211249358</v>
+        <v>0.797696726374305</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>343</v>
+        <v>136</v>
       </c>
       <c r="B14">
-        <v>0.50858225590726702</v>
+        <v>0.55343693962940821</v>
       </c>
       <c r="C14">
-        <v>0.72388709317877842</v>
+        <v>0.79293962940824858</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>391</v>
+        <v>137</v>
       </c>
       <c r="B15">
-        <v>0.51181911613566289</v>
+        <v>0.55060848916592464</v>
       </c>
       <c r="C15">
-        <v>0.74586240251496283</v>
+        <v>0.79887800534283171</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>392</v>
+        <v>141</v>
       </c>
       <c r="B16">
-        <v>0.5125926833752068</v>
+        <v>0.54426629487626343</v>
       </c>
       <c r="C16">
-        <v>0.74856179912984877</v>
+        <v>0.79106599279656098</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>217</v>
+      </c>
+      <c r="B17">
+        <v>0.55319398091223138</v>
+      </c>
+      <c r="C17">
+        <v>0.79426254464547097</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>222</v>
+      </c>
+      <c r="B18">
+        <v>0.54788853777650104</v>
+      </c>
+      <c r="C18">
+        <v>0.79277104280379207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19">
+        <v>223</v>
+      </c>
+      <c r="B19">
+        <v>0.54520015989949167</v>
+      </c>
+      <c r="C19">
+        <v>0.7851584718177147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20">
+        <v>232</v>
+      </c>
+      <c r="B20">
+        <v>0.5499971216395142</v>
+      </c>
+      <c r="C20">
+        <v>0.79624719359852636</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21">
+        <v>233</v>
+      </c>
+      <c r="B21">
+        <v>0.54996282102613969</v>
+      </c>
+      <c r="C21">
+        <v>0.78673053823714467</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>271</v>
+      </c>
+      <c r="B22">
+        <v>0.55030128373067855</v>
+      </c>
+      <c r="C22">
+        <v>0.7908704479958083</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>272</v>
+      </c>
+      <c r="B23">
+        <v>0.55701093719300554</v>
+      </c>
+      <c r="C23">
+        <v>0.80118016896980826</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>273</v>
+      </c>
+      <c r="B24">
+        <v>0.56110534509600418</v>
+      </c>
+      <c r="C24">
+        <v>0.8034723663726</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>274</v>
+      </c>
+      <c r="B25">
+        <v>0.55638426722764067</v>
+      </c>
+      <c r="C25">
+        <v>0.79828902913240263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>275</v>
+      </c>
+      <c r="B26">
+        <v>0.54606083271004735</v>
+      </c>
+      <c r="C26">
+        <v>0.78721515831463484</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>301</v>
+      </c>
+      <c r="B27">
+        <v>0.55296902742158205</v>
+      </c>
+      <c r="C27">
+        <v>0.78940816729137897</v>
       </c>
     </row>
   </sheetData>
@@ -609,7 +726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE946AC8-994E-4D4B-B2E1-65DD3AB691BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55E4F48-806F-4E39-AA48-2BFFEAA7FC4E}">
   <dimension ref="A1:C276"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3654,313 +3771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D5D9F3-3507-4CC3-ABC6-2B1E801F1BE4}">
-  <dimension ref="A1:C27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0.5535201807412834</v>
-      </c>
-      <c r="C3">
-        <v>0.79824204677291311</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>0.55514309663513361</v>
-      </c>
-      <c r="C4">
-        <v>0.79375943000838234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5">
-        <v>39</v>
-      </c>
-      <c r="B5">
-        <v>0.54480670997036007</v>
-      </c>
-      <c r="C5">
-        <v>0.79284543103991922</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6">
-        <v>40</v>
-      </c>
-      <c r="B6">
-        <v>0.55123199999999994</v>
-      </c>
-      <c r="C6">
-        <v>0.79430015999999992</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7">
-        <v>49</v>
-      </c>
-      <c r="B7">
-        <v>0.56088340628730604</v>
-      </c>
-      <c r="C7">
-        <v>0.79514060220188354</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8">
-        <v>50</v>
-      </c>
-      <c r="B8">
-        <v>0.56504494976203068</v>
-      </c>
-      <c r="C8">
-        <v>0.79988696456901109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9">
-        <v>51</v>
-      </c>
-      <c r="B9">
-        <v>0.56937767533750416</v>
-      </c>
-      <c r="C9">
-        <v>0.80036088244978598</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>52</v>
-      </c>
-      <c r="B10">
-        <v>0.57145666710371057</v>
-      </c>
-      <c r="C10">
-        <v>0.79708732135833227</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11">
-        <v>78</v>
-      </c>
-      <c r="B11">
-        <v>0.5711252653927813</v>
-      </c>
-      <c r="C11">
-        <v>0.80882228050455851</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12">
-        <v>113</v>
-      </c>
-      <c r="B12">
-        <v>0.55115106052767715</v>
-      </c>
-      <c r="C12">
-        <v>0.79123706673564398</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13">
-        <v>133</v>
-      </c>
-      <c r="B13">
-        <v>0.56151945645460155</v>
-      </c>
-      <c r="C13">
-        <v>0.797696726374305</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14">
-        <v>136</v>
-      </c>
-      <c r="B14">
-        <v>0.55343693962940821</v>
-      </c>
-      <c r="C14">
-        <v>0.79293962940824858</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15">
-        <v>137</v>
-      </c>
-      <c r="B15">
-        <v>0.55060848916592464</v>
-      </c>
-      <c r="C15">
-        <v>0.79887800534283171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16">
-        <v>141</v>
-      </c>
-      <c r="B16">
-        <v>0.54426629487626343</v>
-      </c>
-      <c r="C16">
-        <v>0.79106599279656098</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A17">
-        <v>217</v>
-      </c>
-      <c r="B17">
-        <v>0.55319398091223138</v>
-      </c>
-      <c r="C17">
-        <v>0.79426254464547097</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18">
-        <v>222</v>
-      </c>
-      <c r="B18">
-        <v>0.54788853777650104</v>
-      </c>
-      <c r="C18">
-        <v>0.79277104280379207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19">
-        <v>223</v>
-      </c>
-      <c r="B19">
-        <v>0.54520015989949167</v>
-      </c>
-      <c r="C19">
-        <v>0.7851584718177147</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20">
-        <v>232</v>
-      </c>
-      <c r="B20">
-        <v>0.5499971216395142</v>
-      </c>
-      <c r="C20">
-        <v>0.79624719359852636</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21">
-        <v>233</v>
-      </c>
-      <c r="B21">
-        <v>0.54996282102613969</v>
-      </c>
-      <c r="C21">
-        <v>0.78673053823714467</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A22">
-        <v>271</v>
-      </c>
-      <c r="B22">
-        <v>0.55030128373067855</v>
-      </c>
-      <c r="C22">
-        <v>0.7908704479958083</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A23">
-        <v>272</v>
-      </c>
-      <c r="B23">
-        <v>0.55701093719300554</v>
-      </c>
-      <c r="C23">
-        <v>0.80118016896980826</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A24">
-        <v>273</v>
-      </c>
-      <c r="B24">
-        <v>0.56110534509600418</v>
-      </c>
-      <c r="C24">
-        <v>0.8034723663726</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A25">
-        <v>274</v>
-      </c>
-      <c r="B25">
-        <v>0.55638426722764067</v>
-      </c>
-      <c r="C25">
-        <v>0.79828902913240263</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A26">
-        <v>275</v>
-      </c>
-      <c r="B26">
-        <v>0.54606083271004735</v>
-      </c>
-      <c r="C26">
-        <v>0.78721515831463484</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A27">
-        <v>301</v>
-      </c>
-      <c r="B27">
-        <v>0.55296902742158205</v>
-      </c>
-      <c r="C27">
-        <v>0.78940816729137897</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA838F4-400B-4E2B-916D-4E788D46E141}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D49248-6EE6-4A31-9F07-29DC71E9D530}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3971,7 +3782,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -4221,8 +4032,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A42400F-F2CB-4BEA-B739-46E2A5151E0E}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C5ACBE-9269-4C89-B2A4-14DB6A956D38}">
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4233,7 +4044,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -4615,8 +4426,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391A80BA-A892-4B8C-9B7A-24C4F6A09584}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40FCC66-E461-46D4-8A6E-83D1A96E061B}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4627,7 +4438,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -4800,8 +4611,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CDD911-80B1-4F1A-98C8-6F765DB56807}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FEDA9E-E230-4466-B1E2-E3E6A3E7A610}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -4812,7 +4623,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Se agregaron las graficas de las interfaces. Se agregaron las constantes de un compuesto (cuadrilatero).
</commit_message>
<xml_diff>
--- a/VerificacionCompuestos/PruebaSalida.xlsx
+++ b/VerificacionCompuestos/PruebaSalida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pamem\OneDrive - UNIVERSIDAD NACIONAL AUTÓNOMA DE MÉXICO\Programación\Matemáticas\Matlab\Proyecto Ana\VerificacionCompuestos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C52FC353-3202-4773-9F38-4DEA9E21934E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F9555647-32C1-486D-8C6F-69BD8D43F654}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16389" windowHeight="12163" firstSheet="2" activeTab="6" xr2:uid="{52623749-0325-4C4F-96ED-C1BE82E86AD0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16389" windowHeight="12163" firstSheet="3" activeTab="7" xr2:uid="{52623749-0325-4C4F-96ED-C1BE82E86AD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="FI2DOLDOLCaCO" sheetId="5" r:id="rId5"/>
     <sheet name="GYPANHDOL" sheetId="6" r:id="rId6"/>
     <sheet name="SalSIL" sheetId="7" r:id="rId7"/>
+    <sheet name="FI2CaCOCaCOSil" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>DOLCALSIL</t>
   </si>
@@ -58,6 +59,9 @@
   </si>
   <si>
     <t>SalSIL</t>
+  </si>
+  <si>
+    <t>FI2CaCOCaCOSil</t>
   </si>
 </sst>
 </file>
@@ -4615,6 +4619,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FEDA9E-E230-4466-B1E2-E3E6A3E7A610}">
   <dimension ref="A1:C2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE52695E-85D2-40FC-B54C-9029BB7241FB}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C2"/>
     </sheetView>
@@ -4623,7 +4658,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -4635,6 +4670,39 @@
       </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>317</v>
+      </c>
+      <c r="B3">
+        <v>0.58297928836962287</v>
+      </c>
+      <c r="C3">
+        <v>0.92219397238449263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>318</v>
+      </c>
+      <c r="B4">
+        <v>0.58411519416210578</v>
+      </c>
+      <c r="C4">
+        <v>0.91104052645295797</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>319</v>
+      </c>
+      <c r="B5">
+        <v>0.57765977621847142</v>
+      </c>
+      <c r="C5">
+        <v>0.88765029395031281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregó un nuevo proyecto sobre ciclos termodinámicos
</commit_message>
<xml_diff>
--- a/VerificacionCompuestos/PruebaSalida.xlsx
+++ b/VerificacionCompuestos/PruebaSalida.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pamem\OneDrive - UNIVERSIDAD NACIONAL AUTÓNOMA DE MÉXICO\Programación\Matemáticas\Matlab\Proyecto Ana\VerificacionCompuestos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{50C131DB-8139-4459-AE49-E138330BB9C6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{037DCDDB-366E-4860-82DB-39B3A2050D44}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16389" windowHeight="12163" firstSheet="7" activeTab="11" xr2:uid="{C876C304-0BBA-4EA1-8714-4A8248379633}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16389" windowHeight="12163" firstSheet="7" activeTab="11" xr2:uid="{A82A682F-2832-48E8-AE27-925134A624BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607824A0-A6C7-437F-8F28-89288FA4FF3E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36A63E5-7DD7-4DF5-A6DF-F2A200C2BB8D}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -506,7 +506,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBE15B6-F21C-47FF-9239-A2897ED8C772}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F6A0A5-37D2-4E5B-A29D-21E630BE5DE9}">
   <dimension ref="A1:D400"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6025,7 +6025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AE1205-4AEB-40EE-8925-D132BBC04544}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDE2142-4AA3-4EFF-9E64-D82BE0F0E73B}">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6392,7 +6392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13EE686C-C195-44C0-A0D9-29629BDB1888}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBD1FEB9-96BA-42A5-9659-2C8359D9634F}">
   <dimension ref="A1:AB401"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -38877,7 +38877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EA4337B-D74B-401F-8523-68E36DD48B4F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DDF351-92A5-482D-A5C0-4DFF85A83546}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -39062,7 +39062,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4BBC7CE-6B52-48C2-8D7C-E04C1B286766}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB11789-EB99-4AF6-8F3A-DB5D8E356F6A}">
   <dimension ref="A1:C277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -42118,7 +42118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4744A907-1541-4079-AC6F-D18FAC8EA8AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA60FE46-895F-454D-BB34-CFC87995CED7}">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -42424,7 +42424,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91E626FA-C35D-4CDD-A9A5-76C60617CE58}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3193F03-2E22-4402-B495-67CBA791688B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -42455,7 +42455,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2A581C-07B1-43F1-9288-97CEA783CAE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34FFA4-7ADD-49EC-B4E5-59D2DA8D9E6C}">
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -42849,7 +42849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4EAE782-C4D0-4FA1-9703-830E85204F5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5529E5-7384-4131-9F6C-7669574AC517}">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -43111,7 +43111,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E2E2E8-297E-4504-92F7-5A22A9756858}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65DC8E61-3964-4DA6-943C-63AB181FE79F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -43142,7 +43142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C2A267-D2E2-45C3-91F6-2D084A3B426A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6710AEDB-DC4C-44BA-90A7-922AEF883B5D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>